<commit_message>
[2020-09-10 17:05] 태그 및 description 유사도
- cloudVec 적용
</commit_message>
<xml_diff>
--- a/dataWork/pre_set/paper/데이터분석+머신러닝+시각화 작업.xlsx
+++ b/dataWork/pre_set/paper/데이터분석+머신러닝+시각화 작업.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\바탕 화면\playdata\ice\py_workspace\Pics\참고자료\자료\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\바탕 화면\playdata\ice\eclipse\Devils_Project\dataWork\pre_set\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1CA003-D858-43DC-8EB3-78C553EA055F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FFD50A-2352-4A18-AD6B-DFCE07995CC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{14B57C06-20CF-49AB-B012-0C25BDF5E9B5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="1" xr2:uid="{14B57C06-20CF-49AB-B012-0C25BDF5E9B5}"/>
   </bookViews>
   <sheets>
     <sheet name="공부 필요한 부분" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>기능 분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -790,6 +790,16 @@
   <si>
     <t>VGG 코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ratsgo.github.io/from%20frequency%20to%20semantics/2017/03/30/word2vec/</t>
+  </si>
+  <si>
+    <t>워드벡(유사단어 추출)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://textmining.kr/?p=416</t>
   </si>
 </sst>
 </file>
@@ -1553,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28E130E-ECDB-41E1-84EF-89B0BFA773C6}">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1663,6 +1673,19 @@
       </c>
       <c r="C16" s="5" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C18" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1679,9 +1702,11 @@
     <hyperlink ref="C14" r:id="rId9" xr:uid="{58DD2524-D37A-4458-8CFA-BCB0CAE89BD9}"/>
     <hyperlink ref="C15" r:id="rId10" xr:uid="{341D20F4-E268-49A7-A16D-7BDF07DCA807}"/>
     <hyperlink ref="C16" r:id="rId11" display="https://minjoos.tistory.com/6" xr:uid="{CA527AED-FFB9-4FF0-B243-C1ED52D386C8}"/>
+    <hyperlink ref="C17" r:id="rId12" display="https://ratsgo.github.io/from frequency to semantics/2017/03/30/word2vec/" xr:uid="{37873897-DB72-49E2-96C6-BC2EED7BF24B}"/>
+    <hyperlink ref="C18" r:id="rId13" xr:uid="{39C82BB2-D2E4-44FA-B25E-D9398E98767E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>